<commit_message>
Fixed some language issues
</commit_message>
<xml_diff>
--- a/Message Varibles.xlsx
+++ b/Message Varibles.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Key</t>
   </si>
@@ -90,19 +90,45 @@
   </si>
   <si>
     <t>PUNISHMENT-IPBAN-KICK</t>
+  </si>
+  <si>
+    <t>PUNISHMENT_MUTE_INFORM</t>
+  </si>
+  <si>
+    <t>Username that was muted</t>
+  </si>
+  <si>
+    <t>PUNISHMENT_MUTE_PLAYER</t>
+  </si>
+  <si>
+    <t>PUNISHMENT_UNMUTE_PLAYER</t>
+  </si>
+  <si>
+    <t>PUNISHMENT_UNMUTE_INFORM</t>
+  </si>
+  <si>
+    <t>Username that was unmuted</t>
+  </si>
+  <si>
+    <t>PUNISHMENT-IPPARDON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,8 +151,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,17 +431,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -523,6 +550,64 @@
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removing Support for tickets; More Lang stuff
</commit_message>
<xml_diff>
--- a/Message Varibles.xlsx
+++ b/Message Varibles.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Key</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>PUNISHMENT-IPPARDON</t>
+  </si>
+  <si>
+    <t>PUNISHMENT-USERPARDON</t>
   </si>
 </sst>
 </file>
@@ -431,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
@@ -594,6 +597,9 @@
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
@@ -606,6 +612,11 @@
       </c>
       <c r="D13" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>